<commit_message>
update figure_BioRECIPE_model_format and update templates
</commit_message>
<xml_diff>
--- a/examples/models/RAS_biorecipes_dynamic_basic.xlsx
+++ b/examples/models/RAS_biorecipes_dynamic_basic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaoxiangzhou/Downloads/BioRECIPES/examples/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743EFF16-4C9E-4C40-B19F-25928C247D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3665959A-CC49-EC40-9D56-16EB28ABEB95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10640" yWindow="1200" windowWidth="28800" windowHeight="15720" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="29">
   <si>
     <t>Element Name</t>
   </si>
@@ -94,6 +94,24 @@
   </si>
   <si>
     <t>Element Database</t>
+  </si>
+  <si>
+    <t>Negative Connection Type</t>
+  </si>
+  <si>
+    <t>Negative Mechanism</t>
+  </si>
+  <si>
+    <t>Negative Site</t>
+  </si>
+  <si>
+    <t>Positive Connection Type</t>
+  </si>
+  <si>
+    <t>Positive Mechanism</t>
+  </si>
+  <si>
+    <t>Positive Site</t>
   </si>
 </sst>
 </file>
@@ -489,18 +507,18 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="24.33203125" style="1"/>
+    <col min="6" max="13" width="24.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -519,11 +537,29 @@
       <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -536,9 +572,15 @@
         <v>6</v>
       </c>
       <c r="F2" s="3"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -551,9 +593,15 @@
         <v>7</v>
       </c>
       <c r="F3" s="4"/>
-      <c r="G3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+    </row>
+    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -568,11 +616,17 @@
       <c r="F4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+    </row>
+    <row r="5" spans="1:13" ht="14.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
@@ -587,9 +641,15 @@
       <c r="F5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+    </row>
+    <row r="6" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -605,8 +665,14 @@
         <v>11</v>
       </c>
       <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+    </row>
+    <row r="7" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -620,8 +686,14 @@
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+    </row>
+    <row r="8" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
@@ -636,11 +708,17 @@
       <c r="F8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+    </row>
+    <row r="9" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
@@ -654,8 +732,14 @@
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+    </row>
+    <row r="10" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
@@ -671,8 +755,14 @@
         <v>19</v>
       </c>
       <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+    </row>
+    <row r="11" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>20</v>
       </c>
@@ -686,8 +776,14 @@
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+    </row>
+    <row r="12" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
@@ -702,11 +798,17 @@
       <c r="F12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+    </row>
+    <row r="13" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>8</v>
       </c>
@@ -722,8 +824,14 @@
         <v>16</v>
       </c>
       <c r="G13" s="6"/>
-    </row>
-    <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+    </row>
+    <row r="14" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6"/>
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
@@ -731,8 +839,14 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
-    </row>
-    <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+    </row>
+    <row r="15" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
@@ -740,8 +854,14 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-    </row>
-    <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+    </row>
+    <row r="16" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
       <c r="B16" s="5"/>
       <c r="C16" s="6"/>
@@ -749,8 +869,14 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
-    </row>
-    <row r="17" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+    </row>
+    <row r="17" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="5"/>
       <c r="C17" s="6"/>
@@ -758,6 +884,12 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>